<commit_message>
Pruebas de favicon failed
</commit_message>
<xml_diff>
--- a/docs/Credenciales.xlsx
+++ b/docs/Credenciales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\garh\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E2F4A2-C42D-4C8C-93F7-17D0AF0FA0E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A344CE72-1614-4D6E-98E7-1DC63C9951D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="11955" yWindow="3150" windowWidth="8535" windowHeight="7770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -516,7 +516,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se actualizó a la versión 1.1
</commit_message>
<xml_diff>
--- a/docs/Credenciales.xlsx
+++ b/docs/Credenciales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\garh\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A344CE72-1614-4D6E-98E7-1DC63C9951D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E222C7F0-2BC6-4BD0-9483-1357AB1C0DCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -516,7 +516,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>